<commit_message>
9 add category to shopping elements (#18)
* Add categories to shopping elements

* Update unit tests

* Fix bad import

* Improve list creation tests

* Add constants for ingredient attributes

* Factorise categorized lists creation
</commit_message>
<xml_diff>
--- a/tests/test_excel_factory/excel_files/add_ingredients.xlsx
+++ b/tests/test_excel_factory/excel_files/add_ingredients.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t xml:space="preserve">Add_ingredients</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">PRIX</t>
   </si>
   <si>
+    <t xml:space="preserve">CATEGORY</t>
+  </si>
+  <si>
     <t xml:space="preserve">UNITE</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Epicerie salee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUPERMARKET</t>
   </si>
   <si>
     <t xml:space="preserve">kg</t>
@@ -258,20 +264,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.56"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -284,47 +293,59 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
+      <c r="D4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="D5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="0" t="n">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <v>0.8</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>